<commit_message>
working version of enhancement
</commit_message>
<xml_diff>
--- a/app/gg_fare_filing.xlsx
+++ b/app/gg_fare_filing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pingsays/git/pingsays/apps/farefiling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pingsays/git/farefiling/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C262296B-0B3A-9342-835B-2A9CBF94B636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2839140D-3D68-484A-9E9B-C11E11A44865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="80">
   <si>
     <t>sort</t>
   </si>
@@ -804,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -891,6 +891,57 @@
       </c>
       <c r="E4" s="3">
         <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>